<commit_message>
Products Approve Excel Updated
</commit_message>
<xml_diff>
--- a/src/assets/samples/ProductsApprove.xlsx
+++ b/src/assets/samples/ProductsApprove.xlsx
@@ -256,31 +256,31 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -362,8 +362,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA2" activeCellId="0" sqref="AA2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -570,7 +570,8 @@
       <c r="AA2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="6" t="b">
+      <c r="AB2" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AC2" s="3" t="s">

</xml_diff>